<commit_message>
minor 5.56 mag update
</commit_message>
<xml_diff>
--- a/changes/556-mags.xlsx
+++ b/changes/556-mags.xlsx
@@ -1,12 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971577E2-4C2E-4039-BDCF-A95183DBD7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="5.56 DRUM Rebalance" sheetId="1" r:id="rId4"/>
+    <sheet name="5.56 DRUM Rebalance" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -229,31 +251,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -261,52 +283,46 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -496,25 +512,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG991"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="44.14"/>
-    <col customWidth="1" min="3" max="33" width="6.71"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="3" max="33" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -552,60 +570,60 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:N2" si="1">CONCAT(P2, "_old")</f>
-        <v>ergonomics_old</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>weight_old</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>horizontal_recoil_old</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>vertical_recoil_old</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>magazine_capacity_old</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>bullet_deviation_old</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>bullet_damage_old</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>bullet_velocity_old</v>
-      </c>
-      <c r="K2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>buck_bullet_deviation_old</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>fire_rate_old</v>
-      </c>
-      <c r="M2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>price_old</v>
-      </c>
-      <c r="N2" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>strength_old</v>
+      <c r="C2" s="1" t="e">
+        <f t="shared" ref="C2:N2" ca="1" si="0">_xludf.CONCAT(P2, "_old")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="I2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="J2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="K2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="L2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="M2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="N2" s="1" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>4</v>
@@ -654,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -662,7 +680,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3">
         <v>0.13</v>
@@ -670,7 +688,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -678,14 +696,14 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="3">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N23" si="2">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300+G3/1.3</f>
-        <v>19.09230769</v>
+        <f t="shared" ref="N3:N23" si="1">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300+G3/1.3</f>
+        <v>19.092307692307692</v>
       </c>
       <c r="P3" s="3">
-        <v>12.0</v>
+        <v>11</v>
       </c>
       <c r="Q3" s="3">
         <v>0.17</v>
@@ -693,7 +711,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
@@ -701,27 +719,27 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="3">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="AA3" s="1">
-        <f t="shared" ref="AA3:AA67" si="3">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*10+W3/300+T3/1.3</f>
-        <v>16.29230769</v>
+        <f t="shared" ref="AA3:AA67" si="2">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*10+W3/300+T3/1.3</f>
+        <v>15.292307692307691</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="5">
         <v>7.2</v>
       </c>
       <c r="AD3" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AE3" s="1">
-        <f t="shared" ref="AE3:AE20" si="4">(AC3*2.5)/100</f>
-        <v>0.18</v>
+        <f>(AC3*2.4)/100</f>
+        <v>0.17280000000000001</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -729,7 +747,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3">
         <v>0.15</v>
@@ -737,7 +755,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -745,14 +763,14 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="3">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="2"/>
-        <v>14.69230769</v>
+        <f t="shared" si="1"/>
+        <v>14.692307692307692</v>
       </c>
       <c r="P4" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="Q4" s="3">
         <v>0.18</v>
@@ -760,7 +778,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
@@ -768,23 +786,23 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="3">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="AA4" s="1">
-        <f t="shared" si="3"/>
-        <v>15.09230769</v>
+        <f t="shared" si="2"/>
+        <v>15.092307692307692</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AE4:AE20" si="3">(AC4*2.4)/100</f>
         <v>0</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -792,7 +810,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>0.25</v>
@@ -800,7 +818,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -808,22 +826,22 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="3">
-        <v>750.0</v>
+        <v>750</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="2"/>
-        <v>13.38461538</v>
+        <f t="shared" si="1"/>
+        <v>13.384615384615383</v>
       </c>
       <c r="P5" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="3">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
@@ -831,27 +849,27 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="3">
-        <v>750.0</v>
+        <v>750</v>
       </c>
       <c r="AA5" s="1">
-        <f t="shared" si="3"/>
-        <v>15.18461538</v>
+        <f t="shared" si="2"/>
+        <v>15.384615384615383</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="2">
         <v>12.5</v>
       </c>
       <c r="AD5" s="2">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AE5" s="1">
-        <f t="shared" si="4"/>
-        <v>0.3125</v>
+        <f t="shared" si="3"/>
+        <v>0.3</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -859,7 +877,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
         <v>0.3</v>
@@ -867,7 +885,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -875,22 +893,22 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="3">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="2"/>
-        <v>14.38461538</v>
+        <f t="shared" si="1"/>
+        <v>14.384615384615383</v>
       </c>
       <c r="P6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="3">
-        <v>0.29</v>
+        <v>0.27</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -898,11 +916,11 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="3">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="AA6" s="1">
-        <f t="shared" si="3"/>
-        <v>14.58461538</v>
+        <f t="shared" si="2"/>
+        <v>14.984615384615383</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="2">
@@ -912,13 +930,13 @@
         <v>2.8</v>
       </c>
       <c r="AE6" s="1">
-        <f t="shared" si="4"/>
-        <v>0.28</v>
+        <f t="shared" si="3"/>
+        <v>0.26879999999999998</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -934,7 +952,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -942,14 +960,14 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="3">
-        <v>750.0</v>
+        <v>750</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="2"/>
-        <v>14.13076923</v>
+        <f t="shared" si="1"/>
+        <v>14.13076923076923</v>
       </c>
       <c r="P7" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="3">
         <v>0.36</v>
@@ -957,7 +975,7 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
@@ -965,23 +983,23 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="3">
-        <v>750.0</v>
+        <v>750</v>
       </c>
       <c r="AA7" s="1">
-        <f t="shared" si="3"/>
-        <v>15.03076923</v>
+        <f t="shared" si="2"/>
+        <v>15.030769230769231</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="3">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D8" s="3">
         <v>0.45</v>
@@ -997,7 +1015,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1005,22 +1023,22 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="3">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="2"/>
-        <v>13.07692308</v>
+        <f t="shared" si="1"/>
+        <v>13.076923076923077</v>
       </c>
       <c r="P8" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="3">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -1028,25 +1046,25 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="3">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="AA8" s="1">
-        <f t="shared" si="3"/>
-        <v>14.67692308</v>
+        <f t="shared" si="2"/>
+        <v>14.876923076923077</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="5">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1">
-        <f t="shared" si="4"/>
-        <v>0.425</v>
+        <f t="shared" si="3"/>
+        <v>0.40799999999999997</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="3">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D9" s="3">
         <v>0.4</v>
@@ -1062,7 +1080,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1070,22 +1088,22 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="3">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="2"/>
-        <v>14.07692308</v>
+        <f t="shared" si="1"/>
+        <v>14.076923076923077</v>
       </c>
       <c r="P9" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="3">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
@@ -1093,27 +1111,27 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="3">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="AA9" s="1">
-        <f t="shared" si="3"/>
-        <v>15.27692308</v>
+        <f t="shared" si="2"/>
+        <v>15.476923076923077</v>
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="2">
         <v>17.7</v>
       </c>
       <c r="AD9" s="2">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="AE9" s="1">
-        <f t="shared" si="4"/>
-        <v>0.4425</v>
+        <f t="shared" si="3"/>
+        <v>0.42479999999999996</v>
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
@@ -1121,7 +1139,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
         <v>0.39</v>
@@ -1129,7 +1147,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1137,22 +1155,22 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="3">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="2"/>
-        <v>16.27692308</v>
+        <f t="shared" si="1"/>
+        <v>16.276923076923076</v>
       </c>
       <c r="P10" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="3">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -1160,23 +1178,23 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="3">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="AA10" s="1">
-        <f t="shared" si="3"/>
-        <v>15.47692308</v>
+        <f t="shared" si="2"/>
+        <v>15.676923076923076</v>
       </c>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -1184,7 +1202,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3">
         <v>0.42</v>
@@ -1192,7 +1210,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1200,22 +1218,22 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="3">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="2"/>
-        <v>14.67692308</v>
+        <f t="shared" si="1"/>
+        <v>14.676923076923076</v>
       </c>
       <c r="P11" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="3">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
@@ -1223,23 +1241,23 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="3">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="AA11" s="1">
-        <f t="shared" si="3"/>
-        <v>15.27692308</v>
+        <f t="shared" si="2"/>
+        <v>15.476923076923077</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="3">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D12" s="3">
         <v>0.42</v>
@@ -1255,7 +1273,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1263,22 +1281,22 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="2"/>
-        <v>13.67692308</v>
+        <f t="shared" si="1"/>
+        <v>13.676923076923076</v>
       </c>
       <c r="P12" s="3">
         <v>1.5</v>
       </c>
       <c r="Q12" s="3">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
@@ -1286,23 +1304,23 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="1">
-        <f t="shared" si="3"/>
-        <v>15.37692308</v>
+        <f t="shared" si="2"/>
+        <v>15.576923076923077</v>
       </c>
       <c r="AB12" s="1"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -1318,7 +1336,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1326,22 +1344,22 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="3">
-        <v>1300.0</v>
+        <v>1300</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="2"/>
-        <v>13.17692308</v>
+        <f t="shared" si="1"/>
+        <v>13.176923076923076</v>
       </c>
       <c r="P13" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="3">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
@@ -1349,28 +1367,28 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="3">
-        <v>1300.0</v>
+        <v>1300</v>
       </c>
       <c r="AA13" s="1">
-        <f t="shared" si="3"/>
-        <v>14.87692308</v>
+        <f t="shared" si="2"/>
+        <v>15.076923076923077</v>
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="6">
-        <f t="shared" ref="AC13:AC14" si="5">AD13+17.7-5.1</f>
-        <v>18.6</v>
+        <f t="shared" ref="AC13:AC14" si="4">AD13+17.7-5.1</f>
+        <v>18.600000000000001</v>
       </c>
       <c r="AD13" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AE13" s="1">
-        <f t="shared" si="4"/>
-        <v>0.465</v>
+        <f t="shared" si="3"/>
+        <v>0.44640000000000002</v>
       </c>
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -1378,7 +1396,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="3">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="D14" s="3">
         <v>0.46</v>
@@ -1386,7 +1404,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1394,22 +1412,22 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="3">
-        <v>1200.0</v>
+        <v>1200</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="2"/>
-        <v>12.87692308</v>
+        <f t="shared" si="1"/>
+        <v>12.876923076923076</v>
       </c>
       <c r="P14" s="3">
         <v>0.5</v>
       </c>
       <c r="Q14" s="3">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
@@ -1417,28 +1435,28 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
       <c r="Z14" s="3">
-        <v>1200.0</v>
+        <v>1200</v>
       </c>
       <c r="AA14" s="1">
-        <f t="shared" si="3"/>
-        <v>14.97692308</v>
+        <f t="shared" si="2"/>
+        <v>15.176923076923076</v>
       </c>
       <c r="AB14" s="1"/>
       <c r="AC14" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>21.4</v>
       </c>
       <c r="AD14" s="2">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AE14" s="1">
-        <f t="shared" si="4"/>
-        <v>0.535</v>
+        <f t="shared" si="3"/>
+        <v>0.51359999999999995</v>
       </c>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -1446,15 +1464,15 @@
         <v>44</v>
       </c>
       <c r="C15" s="3">
-        <v>-10.0</v>
+        <v>-10</v>
       </c>
       <c r="D15" s="3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1462,22 +1480,22 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="3">
-        <v>1600.0</v>
+        <v>1600</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="2"/>
-        <v>9.769230769</v>
+        <f t="shared" si="1"/>
+        <v>9.7692307692307665</v>
       </c>
       <c r="P15" s="3">
-        <v>-6.0</v>
+        <v>-6</v>
       </c>
       <c r="Q15" s="3">
-        <v>0.58</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
@@ -1485,27 +1503,27 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="3">
-        <v>1600.0</v>
+        <v>1600</v>
       </c>
       <c r="AA15" s="1">
+        <f t="shared" si="2"/>
+        <v>13.369230769230768</v>
+      </c>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1">
+        <v>23.1</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="AE15" s="1">
         <f t="shared" si="3"/>
-        <v>13.16923077</v>
-      </c>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="2">
-        <v>23.1</v>
-      </c>
-      <c r="AD15" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="AE15" s="1">
-        <f t="shared" si="4"/>
-        <v>0.5775</v>
+        <v>0.5544</v>
       </c>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1513,15 +1531,15 @@
         <v>46</v>
       </c>
       <c r="C16" s="3">
-        <v>-6.0</v>
+        <v>-6</v>
       </c>
       <c r="D16" s="3">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="3">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1529,14 +1547,14 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="3">
-        <v>1600.0</v>
+        <v>1600</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="2"/>
-        <v>14.90769231</v>
+        <f t="shared" si="1"/>
+        <v>14.907692307692308</v>
       </c>
       <c r="P16" s="3">
-        <v>-7.0</v>
+        <v>-6</v>
       </c>
       <c r="Q16" s="3">
         <v>0.6</v>
@@ -1544,7 +1562,7 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="3">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
@@ -1552,23 +1570,23 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="3">
-        <v>1600.0</v>
+        <v>1600</v>
       </c>
       <c r="AA16" s="1">
-        <f t="shared" si="3"/>
-        <v>13.30769231</v>
+        <f t="shared" si="2"/>
+        <v>14.307692307692307</v>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="2"/>
+      <c r="AD16" s="1"/>
       <c r="AE16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -1576,7 +1594,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="3">
-        <v>-7.0</v>
+        <v>-7</v>
       </c>
       <c r="D17" s="3">
         <v>0.61</v>
@@ -1584,7 +1602,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1592,22 +1610,22 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="3">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="2"/>
-        <v>19.26153846</v>
+        <f t="shared" si="1"/>
+        <v>19.261538461538461</v>
       </c>
       <c r="P17" s="3">
-        <v>-8.0</v>
+        <v>-8</v>
       </c>
       <c r="Q17" s="3">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="U17" s="3">
         <v>0.1</v>
@@ -1617,27 +1635,27 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
       <c r="Z17" s="3">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="AA17" s="1">
+        <f t="shared" si="2"/>
+        <v>8.9615384615384599</v>
+      </c>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1">
+        <v>43</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE17" s="1">
         <f t="shared" si="3"/>
-        <v>8.561538462</v>
-      </c>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="2">
-        <v>43.0</v>
-      </c>
-      <c r="AD17" s="2">
-        <v>23.0</v>
-      </c>
-      <c r="AE17" s="1">
-        <f t="shared" si="4"/>
-        <v>1.075</v>
+        <v>1.032</v>
       </c>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
@@ -1645,7 +1663,7 @@
         <v>50</v>
       </c>
       <c r="C18" s="3">
-        <v>-10.0</v>
+        <v>-10</v>
       </c>
       <c r="D18" s="3">
         <v>0.9</v>
@@ -1653,7 +1671,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="H18" s="3">
         <v>0.1</v>
@@ -1663,22 +1681,22 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="3">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="2"/>
-        <v>17.65384615</v>
+        <f t="shared" si="1"/>
+        <v>17.653846153846153</v>
       </c>
       <c r="P18" s="3">
-        <v>-12.0</v>
+        <v>-12</v>
       </c>
       <c r="Q18" s="3">
-        <v>1.15</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="U18" s="3">
         <v>0.1</v>
@@ -1688,27 +1706,27 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="3">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="AA18" s="1">
+        <f t="shared" si="2"/>
+        <v>11.253846153846148</v>
+      </c>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1">
+        <v>46</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="AE18" s="1">
         <f t="shared" si="3"/>
-        <v>10.65384615</v>
-      </c>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="7">
-        <v>46.0</v>
-      </c>
-      <c r="AD18" s="2">
-        <v>20.5</v>
-      </c>
-      <c r="AE18" s="1">
-        <f t="shared" si="4"/>
-        <v>1.15</v>
+        <v>1.1039999999999999</v>
       </c>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -1716,7 +1734,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="3">
-        <v>-9.0</v>
+        <v>-9</v>
       </c>
       <c r="D19" s="3">
         <v>0.82</v>
@@ -1724,7 +1742,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="H19" s="3">
         <v>0.1</v>
@@ -1734,22 +1752,22 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="3">
-        <v>3500.0</v>
+        <v>3500</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="2"/>
-        <v>20.25384615</v>
+        <f t="shared" si="1"/>
+        <v>20.253846153846155</v>
       </c>
       <c r="P19" s="3">
-        <v>-16.0</v>
+        <v>-17</v>
       </c>
       <c r="Q19" s="3">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="U19" s="3">
         <v>0.1</v>
@@ -1759,27 +1777,27 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="3">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="AA19" s="1">
+        <f t="shared" si="2"/>
+        <v>11.253846153846155</v>
+      </c>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="AE19" s="1">
         <f t="shared" si="3"/>
-        <v>11.65384615</v>
-      </c>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="2">
-        <v>35.2</v>
-      </c>
-      <c r="AD19" s="2">
-        <v>6.4</v>
-      </c>
-      <c r="AE19" s="1">
-        <f t="shared" si="4"/>
-        <v>0.88</v>
+        <v>0.8448</v>
       </c>
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
@@ -1787,15 +1805,15 @@
         <v>54</v>
       </c>
       <c r="C20" s="3">
-        <v>-16.0</v>
+        <v>-16</v>
       </c>
       <c r="D20" s="3">
-        <v>1.16</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="H20" s="3">
         <v>0.15</v>
@@ -1805,22 +1823,22 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="3">
-        <v>6000.0</v>
+        <v>6000</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="2"/>
-        <v>36.97307692</v>
+        <f t="shared" si="1"/>
+        <v>36.973076923076917</v>
       </c>
       <c r="P20" s="3">
-        <v>-25.0</v>
+        <v>-26</v>
       </c>
       <c r="Q20" s="3">
-        <v>1.32</v>
+        <v>1.29</v>
       </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="U20" s="3">
         <v>0.15</v>
@@ -1830,27 +1848,27 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="3">
-        <v>5500.0</v>
+        <v>5500</v>
       </c>
       <c r="AA20" s="1">
+        <f t="shared" si="2"/>
+        <v>24.373076923076923</v>
+      </c>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1">
+        <v>52.8</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="AE20" s="1">
         <f t="shared" si="3"/>
-        <v>24.77307692</v>
-      </c>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="2">
-        <v>52.8</v>
-      </c>
-      <c r="AD20" s="2">
-        <v>9.6</v>
-      </c>
-      <c r="AE20" s="1">
-        <f t="shared" si="4"/>
-        <v>1.32</v>
+        <v>1.2671999999999999</v>
       </c>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1865,7 +1883,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21" s="4"/>
@@ -1880,7 +1898,7 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB21" s="1"/>
@@ -1890,7 +1908,7 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1898,7 +1916,7 @@
         <v>56</v>
       </c>
       <c r="C22" s="3">
-        <v>-2.0</v>
+        <v>-2</v>
       </c>
       <c r="D22" s="3">
         <v>0.06</v>
@@ -1906,7 +1924,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1914,14 +1932,14 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="3">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="2"/>
-        <v>0.6461538462</v>
+        <f t="shared" si="1"/>
+        <v>0.64615384615384563</v>
       </c>
       <c r="P22" s="3">
-        <v>-2.0</v>
+        <v>-2</v>
       </c>
       <c r="Q22" s="3">
         <v>0.08</v>
@@ -1929,7 +1947,7 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
@@ -1937,11 +1955,11 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
       <c r="Z22" s="3">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="AA22" s="1">
-        <f t="shared" si="3"/>
-        <v>0.2461538462</v>
+        <f t="shared" si="2"/>
+        <v>0.24615384615384572</v>
       </c>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
@@ -1950,7 +1968,7 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
@@ -1958,10 +1976,10 @@
         <v>58</v>
       </c>
       <c r="C23" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1972,14 +1990,14 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="P23" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="3">
         <v>0.02</v>
@@ -1993,10 +2011,10 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="AB23" s="1"/>
@@ -2006,7 +2024,7 @@
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>59</v>
       </c>
@@ -2014,10 +2032,10 @@
         <v>60</v>
       </c>
       <c r="C24" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2028,11 +2046,11 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1"/>
       <c r="P24" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="3">
         <v>0.02</v>
@@ -2046,10 +2064,10 @@
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
       <c r="Z24" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="AB24" s="1"/>
@@ -2059,7 +2077,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -2067,7 +2085,7 @@
         <v>62</v>
       </c>
       <c r="C25" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
         <v>0.02</v>
@@ -2081,14 +2099,14 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" ref="N25:N67" si="6">C25-D25*20-E25*0.8-F25*0.6-H25*5+I25*10+J25/300+G25/1.3</f>
+        <f t="shared" ref="N25:N67" si="5">C25-D25*20-E25*0.8-F25*0.6-H25*5+I25*10+J25/300+G25/1.3</f>
         <v>0.6</v>
       </c>
       <c r="P25" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="3">
         <v>0.02</v>
@@ -2102,10 +2120,10 @@
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
       <c r="Z25" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="AB25" s="1"/>
@@ -2115,7 +2133,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>63</v>
       </c>
@@ -2123,7 +2141,7 @@
         <v>64</v>
       </c>
       <c r="C26" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="3">
         <v>0.03</v>
@@ -2137,14 +2155,14 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="3">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.4</v>
       </c>
       <c r="P26" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="Q26" s="3">
         <v>0.04</v>
@@ -2158,10 +2176,10 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="3">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="AA26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
       <c r="AB26" s="1"/>
@@ -2171,7 +2189,7 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
@@ -2179,10 +2197,10 @@
         <v>66</v>
       </c>
       <c r="C27" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2193,14 +2211,14 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="P27" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="3">
         <v>0.02</v>
@@ -2214,10 +2232,10 @@
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
       <c r="Z27" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="AB27" s="1"/>
@@ -2227,7 +2245,7 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>67</v>
       </c>
@@ -2235,7 +2253,7 @@
         <v>68</v>
       </c>
       <c r="C28" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D28" s="3">
         <v>0.01</v>
@@ -2249,14 +2267,14 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-0.2</v>
       </c>
       <c r="P28" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="3">
         <v>0.02</v>
@@ -2270,10 +2288,10 @@
       <c r="X28" s="4"/>
       <c r="Y28" s="4"/>
       <c r="Z28" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="AB28" s="1"/>
@@ -2283,7 +2301,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
@@ -2291,7 +2309,7 @@
         <v>70</v>
       </c>
       <c r="C29" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="3">
         <v>0.02</v>
@@ -2305,14 +2323,14 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="P29" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="3">
         <v>0.02</v>
@@ -2326,10 +2344,10 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AA29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="AB29" s="1"/>
@@ -2339,7 +2357,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2354,7 +2372,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P30" s="4"/>
@@ -2369,7 +2387,7 @@
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
       <c r="AA30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB30" s="1"/>
@@ -2379,13 +2397,13 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N31" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB31" s="1"/>
@@ -2395,13 +2413,13 @@
       <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N32" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB32" s="1"/>
@@ -2411,13 +2429,13 @@
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB33" s="1"/>
@@ -2427,13 +2445,13 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB34" s="1"/>
@@ -2443,13 +2461,13 @@
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB35" s="1"/>
@@ -2459,13 +2477,13 @@
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N36" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB36" s="1"/>
@@ -2475,13 +2493,13 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N37" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB37" s="1"/>
@@ -2491,13 +2509,13 @@
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N38" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB38" s="1"/>
@@ -2507,13 +2525,13 @@
       <c r="AF38" s="1"/>
       <c r="AG38" s="1"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N39" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB39" s="1"/>
@@ -2523,13 +2541,13 @@
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N40" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB40" s="1"/>
@@ -2539,13 +2557,13 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N41" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB41" s="1"/>
@@ -2555,13 +2573,13 @@
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB42" s="1"/>
@@ -2571,13 +2589,13 @@
       <c r="AF42" s="1"/>
       <c r="AG42" s="1"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N43" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB43" s="1"/>
@@ -2587,13 +2605,13 @@
       <c r="AF43" s="1"/>
       <c r="AG43" s="1"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N44" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB44" s="1"/>
@@ -2603,13 +2621,13 @@
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB45" s="1"/>
@@ -2619,13 +2637,13 @@
       <c r="AF45" s="1"/>
       <c r="AG45" s="1"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N46" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB46" s="1"/>
@@ -2635,13 +2653,13 @@
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N47" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB47" s="1"/>
@@ -2651,13 +2669,13 @@
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N48" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB48" s="1"/>
@@ -2667,13 +2685,13 @@
       <c r="AF48" s="1"/>
       <c r="AG48" s="1"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N49" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB49" s="1"/>
@@ -2683,13 +2701,13 @@
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N50" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB50" s="1"/>
@@ -2699,13 +2717,13 @@
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N51" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB51" s="1"/>
@@ -2715,13 +2733,13 @@
       <c r="AF51" s="1"/>
       <c r="AG51" s="1"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N52" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB52" s="1"/>
@@ -2731,13 +2749,13 @@
       <c r="AF52" s="1"/>
       <c r="AG52" s="1"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N53" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB53" s="1"/>
@@ -2747,13 +2765,13 @@
       <c r="AF53" s="1"/>
       <c r="AG53" s="1"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N54" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB54" s="1"/>
@@ -2763,13 +2781,13 @@
       <c r="AF54" s="1"/>
       <c r="AG54" s="1"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N55" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB55" s="1"/>
@@ -2779,13 +2797,13 @@
       <c r="AF55" s="1"/>
       <c r="AG55" s="1"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N56" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB56" s="1"/>
@@ -2795,13 +2813,13 @@
       <c r="AF56" s="1"/>
       <c r="AG56" s="1"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N57" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB57" s="1"/>
@@ -2811,13 +2829,13 @@
       <c r="AF57" s="1"/>
       <c r="AG57" s="1"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N58" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB58" s="1"/>
@@ -2827,13 +2845,13 @@
       <c r="AF58" s="1"/>
       <c r="AG58" s="1"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB59" s="1"/>
@@ -2843,13 +2861,13 @@
       <c r="AF59" s="1"/>
       <c r="AG59" s="1"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA60" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB60" s="1"/>
@@ -2859,13 +2877,13 @@
       <c r="AF60" s="1"/>
       <c r="AG60" s="1"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N61" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA61" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB61" s="1"/>
@@ -2875,13 +2893,13 @@
       <c r="AF61" s="1"/>
       <c r="AG61" s="1"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N62" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA62" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB62" s="1"/>
@@ -2891,13 +2909,13 @@
       <c r="AF62" s="1"/>
       <c r="AG62" s="1"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N63" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA63" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB63" s="1"/>
@@ -2907,13 +2925,13 @@
       <c r="AF63" s="1"/>
       <c r="AG63" s="1"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N64" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA64" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB64" s="1"/>
@@ -2923,13 +2941,13 @@
       <c r="AF64" s="1"/>
       <c r="AG64" s="1"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N65" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA65" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB65" s="1"/>
@@ -2939,13 +2957,13 @@
       <c r="AF65" s="1"/>
       <c r="AG65" s="1"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N66" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA66" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB66" s="1"/>
@@ -2955,13 +2973,13 @@
       <c r="AF66" s="1"/>
       <c r="AG66" s="1"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N67" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA67" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB67" s="1"/>
@@ -2971,934 +2989,932 @@
       <c r="AF67" s="1"/>
       <c r="AG67" s="1"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="68" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add l5awm mag and fix some weights
</commit_message>
<xml_diff>
--- a/changes/556-mags.xlsx
+++ b/changes/556-mags.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971577E2-4C2E-4039-BDCF-A95183DBD7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEF4CA5F-D521-417C-BB27-96ADE0BE323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="5.56 DRUM Rebalance" sheetId="1" r:id="rId1"/>
+    <sheet name="556-mags" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>old</t>
   </si>
@@ -246,13 +246,31 @@
   </si>
   <si>
     <t>HK Mag Bottom Plate</t>
+  </si>
+  <si>
+    <t>5.56x45_lancer_systems_l5awm_gen2_30r_opaque_mag</t>
+  </si>
+  <si>
+    <t>5.56x45_lancer_systems_l5awm_gen2_30r_translucent_mag</t>
+  </si>
+  <si>
+    <t>Lancer Systems L5AWM Gen2 30R Opaque</t>
+  </si>
+  <si>
+    <t>Lancer Systems L5AWM Gen2 30R Translucent</t>
+  </si>
+  <si>
+    <t>lancer_systems_l5awm_gen2_bottom_plate</t>
+  </si>
+  <si>
+    <t>Lancer Systems L5AWM Gen2 Bottom Plate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +286,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -296,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -304,6 +328,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,15 +545,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG991"/>
+  <dimension ref="A1:AG994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.140625" customWidth="1"/>
     <col min="3" max="33" width="6.7109375" customWidth="1"/>
   </cols>
@@ -699,14 +725,14 @@
         <v>500</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N23" si="1">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300+G3/1.3</f>
+        <f t="shared" ref="N3:N26" si="1">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300+G3/1.3</f>
         <v>19.092307692307692</v>
       </c>
       <c r="P3" s="3">
         <v>11</v>
       </c>
       <c r="Q3" s="3">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -722,8 +748,8 @@
         <v>500</v>
       </c>
       <c r="AA3" s="1">
-        <f t="shared" ref="AA3:AA67" si="2">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*10+W3/300+T3/1.3</f>
-        <v>15.292307692307691</v>
+        <f t="shared" ref="AA3:AA70" si="2">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*10+W3/300+T3/1.3</f>
+        <v>15.692307692307692</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="5">
@@ -773,7 +799,7 @@
         <v>11</v>
       </c>
       <c r="Q4" s="3">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
@@ -790,13 +816,13 @@
       </c>
       <c r="AA4" s="1">
         <f t="shared" si="2"/>
-        <v>15.092307692307692</v>
+        <v>15.492307692307691</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="1">
-        <f t="shared" ref="AE4:AE20" si="3">(AC4*2.4)/100</f>
+        <f t="shared" ref="AE4:AE23" si="3">(AC4*2.4)/100</f>
         <v>0</v>
       </c>
       <c r="AF4" s="1"/>
@@ -836,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="Q5" s="3">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
@@ -853,7 +879,7 @@
       </c>
       <c r="AA5" s="1">
         <f t="shared" si="2"/>
-        <v>15.384615384615383</v>
+        <v>15.784615384615382</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="2">
@@ -903,7 +929,7 @@
         <v>5</v>
       </c>
       <c r="Q6" s="3">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -920,7 +946,7 @@
       </c>
       <c r="AA6" s="1">
         <f t="shared" si="2"/>
-        <v>14.984615384615383</v>
+        <v>15.384615384615383</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="2">
@@ -970,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="Q7" s="3">
-        <v>0.36</v>
+        <v>0.34</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -987,7 +1013,7 @@
       </c>
       <c r="AA7" s="1">
         <f t="shared" si="2"/>
-        <v>15.030769230769231</v>
+        <v>15.430769230769229</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
@@ -1033,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="3">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1050,7 +1076,7 @@
       </c>
       <c r="AA8" s="1">
         <f t="shared" si="2"/>
-        <v>14.876923076923077</v>
+        <v>15.276923076923076</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="5">
@@ -1098,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="3">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1115,7 +1141,7 @@
       </c>
       <c r="AA9" s="1">
         <f t="shared" si="2"/>
-        <v>15.476923076923077</v>
+        <v>15.876923076923077</v>
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="2">
@@ -1165,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="3">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -1182,7 +1208,7 @@
       </c>
       <c r="AA10" s="1">
         <f t="shared" si="2"/>
-        <v>15.676923076923076</v>
+        <v>16.076923076923077</v>
       </c>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -1228,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="Q11" s="3">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -1245,7 +1271,7 @@
       </c>
       <c r="AA11" s="1">
         <f t="shared" si="2"/>
-        <v>15.476923076923077</v>
+        <v>15.876923076923077</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
@@ -1291,7 +1317,7 @@
         <v>1.5</v>
       </c>
       <c r="Q12" s="3">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1308,7 +1334,7 @@
       </c>
       <c r="AA12" s="1">
         <f t="shared" si="2"/>
-        <v>15.576923076923077</v>
+        <v>15.776923076923076</v>
       </c>
       <c r="AB12" s="1"/>
       <c r="AC12" s="5"/>
@@ -1354,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="Q13" s="3">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -1371,7 +1397,7 @@
       </c>
       <c r="AA13" s="1">
         <f t="shared" si="2"/>
-        <v>15.076923076923077</v>
+        <v>15.476923076923077</v>
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="6">
@@ -1419,7 +1445,7 @@
         <v>12.876923076923076</v>
       </c>
       <c r="P14" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="3">
         <v>0.42</v>
@@ -1439,7 +1465,7 @@
       </c>
       <c r="AA14" s="1">
         <f t="shared" si="2"/>
-        <v>15.176923076923076</v>
+        <v>15.676923076923076</v>
       </c>
       <c r="AB14" s="1"/>
       <c r="AC14" s="6">
@@ -1456,46 +1482,34 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="3">
-        <v>-10</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.55000000000000004</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="3">
-        <v>40</v>
-      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="3">
-        <v>1600</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="1"/>
-        <v>9.7692307692307665</v>
-      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="1"/>
       <c r="P15" s="3">
-        <v>-6</v>
+        <v>-1.5</v>
       </c>
       <c r="Q15" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
@@ -1503,66 +1517,54 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="3">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="AA15" s="1">
         <f t="shared" si="2"/>
-        <v>13.369230769230768</v>
+        <v>15.976923076923075</v>
       </c>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="1">
-        <v>23.1</v>
-      </c>
-      <c r="AD15" s="1">
-        <v>6.2</v>
+      <c r="AC15" s="8">
+        <v>12.5</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>3.8</v>
       </c>
       <c r="AE15" s="1">
         <f t="shared" si="3"/>
-        <v>0.5544</v>
+        <v>0.3</v>
       </c>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
     </row>
     <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="3">
-        <v>-6</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.56999999999999995</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="3">
-        <v>42</v>
-      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="3">
-        <v>1600</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="1"/>
-        <v>14.907692307692308</v>
-      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="1"/>
       <c r="P16" s="3">
-        <v>-6</v>
+        <v>-1.5</v>
       </c>
       <c r="Q16" s="3">
-        <v>0.6</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="3">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
@@ -1570,473 +1572,473 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="3">
-        <v>1600</v>
+        <v>1700</v>
       </c>
       <c r="AA16" s="1">
         <f t="shared" si="2"/>
-        <v>14.307692307692307</v>
+        <v>15.976923076923075</v>
       </c>
       <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="3">
-        <v>-7</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.61</v>
-      </c>
+    <row r="17" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="3">
-        <v>50</v>
-      </c>
+      <c r="G17" s="3"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="3">
-        <v>3000</v>
-      </c>
-      <c r="N17" s="1">
-        <f t="shared" si="1"/>
-        <v>19.261538461538461</v>
-      </c>
-      <c r="P17" s="3">
-        <v>-8</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1.05</v>
-      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="3">
-        <v>50</v>
-      </c>
-      <c r="U17" s="3">
-        <v>0.1</v>
-      </c>
+      <c r="T17" s="3"/>
+      <c r="U17" s="4"/>
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="3">
-        <v>3000</v>
-      </c>
+      <c r="Z17" s="3"/>
       <c r="AA17" s="1">
         <f t="shared" si="2"/>
-        <v>8.9615384615384599</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="1">
-        <v>43</v>
-      </c>
-      <c r="AD17" s="1">
-        <v>23</v>
-      </c>
-      <c r="AE17" s="1">
-        <f t="shared" si="3"/>
-        <v>1.032</v>
-      </c>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3">
         <v>-10</v>
       </c>
       <c r="D18" s="3">
-        <v>0.9</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3">
-        <v>60</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="3">
-        <v>4000</v>
+        <v>1600</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="1"/>
-        <v>17.653846153846153</v>
+        <v>9.7692307692307665</v>
       </c>
       <c r="P18" s="3">
-        <v>-12</v>
+        <v>-6</v>
       </c>
       <c r="Q18" s="3">
-        <v>1.1200000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="3">
-        <v>60</v>
-      </c>
-      <c r="U18" s="3">
-        <v>0.1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="3">
-        <v>4000</v>
+        <v>1600</v>
       </c>
       <c r="AA18" s="1">
         <f t="shared" si="2"/>
-        <v>11.253846153846148</v>
+        <v>13.969230769230766</v>
       </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1">
-        <v>46</v>
+        <v>23.1</v>
       </c>
       <c r="AD18" s="1">
-        <v>20.5</v>
+        <v>6.2</v>
       </c>
       <c r="AE18" s="1">
         <f t="shared" si="3"/>
-        <v>1.1039999999999999</v>
+        <v>0.5544</v>
       </c>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3">
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="D19" s="3">
-        <v>0.82</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="3">
-        <v>60</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0.1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="3">
-        <v>3500</v>
+        <v>1600</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="1"/>
-        <v>20.253846153846155</v>
+        <v>14.907692307692308</v>
       </c>
       <c r="P19" s="3">
-        <v>-17</v>
+        <v>-6</v>
       </c>
       <c r="Q19" s="3">
-        <v>0.87</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="3">
-        <v>60</v>
-      </c>
-      <c r="U19" s="3">
-        <v>0.1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="3">
-        <v>4000</v>
+        <v>1600</v>
       </c>
       <c r="AA19" s="1">
         <f t="shared" si="2"/>
-        <v>11.253846153846155</v>
+        <v>14.707692307692305</v>
       </c>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="1">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="AD19" s="1">
-        <v>6.4</v>
-      </c>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
       <c r="AE19" s="1">
         <f t="shared" si="3"/>
-        <v>0.8448</v>
+        <v>0</v>
       </c>
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
     </row>
-    <row r="20" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3">
-        <v>-16</v>
+        <v>-7</v>
       </c>
       <c r="D20" s="3">
-        <v>1.1599999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="3">
-        <v>100</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.15</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="3">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" si="1"/>
-        <v>36.973076923076917</v>
+        <v>19.261538461538461</v>
       </c>
       <c r="P20" s="3">
-        <v>-26</v>
+        <v>-8</v>
       </c>
       <c r="Q20" s="3">
-        <v>1.29</v>
+        <v>1.05</v>
       </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="U20" s="3">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="3">
-        <v>5500</v>
+        <v>3000</v>
       </c>
       <c r="AA20" s="1">
         <f t="shared" si="2"/>
-        <v>24.373076923076923</v>
+        <v>8.9615384615384599</v>
       </c>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1">
-        <v>52.8</v>
+        <v>43</v>
       </c>
       <c r="AD20" s="1">
-        <v>9.6</v>
+        <v>23</v>
       </c>
       <c r="AE20" s="1">
         <f t="shared" si="3"/>
-        <v>1.2671999999999999</v>
+        <v>1.032</v>
       </c>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3">
+        <v>-10</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.9</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="G21" s="3">
+        <v>60</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.1</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="M21" s="3">
+        <v>4000</v>
+      </c>
       <c r="N21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
+        <v>17.653846153846153</v>
+      </c>
+      <c r="P21" s="3">
+        <v>-12</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1.1200000000000001</v>
+      </c>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
+      <c r="T21" s="3">
+        <v>60</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0.1</v>
+      </c>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
+      <c r="Z21" s="3">
+        <v>4000</v>
+      </c>
       <c r="AA21" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.253846153846148</v>
       </c>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="1"/>
+      <c r="AC21" s="1">
+        <v>46</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="AE21" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1039999999999999</v>
+      </c>
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
     </row>
     <row r="22" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3">
-        <v>-2</v>
+        <v>-9</v>
       </c>
       <c r="D22" s="3">
-        <v>0.06</v>
+        <v>0.82</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="3">
-        <v>5</v>
-      </c>
-      <c r="H22" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.1</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="3">
-        <v>400</v>
+        <v>3500</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="1"/>
-        <v>0.64615384615384563</v>
+        <v>20.253846153846155</v>
       </c>
       <c r="P22" s="3">
-        <v>-2</v>
+        <v>-17</v>
       </c>
       <c r="Q22" s="3">
-        <v>0.08</v>
+        <v>0.87</v>
       </c>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="3">
-        <v>5</v>
-      </c>
-      <c r="U22" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0.1</v>
+      </c>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
       <c r="Z22" s="3">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="AA22" s="1">
         <f t="shared" si="2"/>
-        <v>0.24615384615384572</v>
+        <v>11.253846153846155</v>
       </c>
       <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="1"/>
+      <c r="AC22" s="1">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="AE22" s="1">
+        <f t="shared" si="3"/>
+        <v>0.8448</v>
+      </c>
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
     </row>
     <row r="23" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3">
-        <v>1</v>
+        <v>-16</v>
       </c>
       <c r="D23" s="3">
-        <v>1.4999999999999999E-2</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="G23" s="3">
+        <v>100</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.15</v>
+      </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="3">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="N23" s="1">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>36.973076923076917</v>
       </c>
       <c r="P23" s="3">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="Q23" s="3">
-        <v>0.02</v>
+        <v>1.29</v>
       </c>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
+      <c r="T23" s="3">
+        <v>100</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0.15</v>
+      </c>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
       <c r="Z23" s="3">
-        <v>0</v>
+        <v>5500</v>
       </c>
       <c r="AA23" s="1">
         <f t="shared" si="2"/>
-        <v>-0.4</v>
+        <v>25.373076923076923</v>
       </c>
       <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-      <c r="AE23" s="1"/>
+      <c r="AC23" s="1">
+        <v>52.8</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="AE23" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2671999999999999</v>
+      </c>
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
     </row>
     <row r="24" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1.4999999999999999E-2</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2045,16 +2047,13 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="3">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1"/>
-      <c r="P24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="3">
-        <v>0.02</v>
-      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
@@ -2063,12 +2062,10 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
-      <c r="Z24" s="3">
-        <v>0</v>
-      </c>
+      <c r="Z24" s="4"/>
       <c r="AA24" s="1">
         <f t="shared" si="2"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
@@ -2079,52 +2076,56 @@
     </row>
     <row r="25" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C25" s="3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D25" s="3">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="G25" s="3">
+        <v>5</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="3">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" ref="N25:N67" si="5">C25-D25*20-E25*0.8-F25*0.6-H25*5+I25*10+J25/300+G25/1.3</f>
-        <v>0.6</v>
+        <f t="shared" si="1"/>
+        <v>0.64615384615384563</v>
       </c>
       <c r="P25" s="3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Q25" s="3">
-        <v>0.02</v>
+        <v>0.08</v>
       </c>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
+      <c r="T25" s="3">
+        <v>5</v>
+      </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
       <c r="Z25" s="3">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="AA25" s="1">
         <f t="shared" si="2"/>
-        <v>-0.4</v>
+        <v>0.24615384615384572</v>
       </c>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
@@ -2135,16 +2136,16 @@
     </row>
     <row r="26" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C26" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2155,17 +2156,17 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="5"/>
-        <v>1.4</v>
+        <f t="shared" si="1"/>
+        <v>0.7</v>
       </c>
       <c r="P26" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="3">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
@@ -2176,11 +2177,11 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AA26" s="1">
         <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>-0.4</v>
       </c>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
@@ -2191,10 +2192,10 @@
     </row>
     <row r="27" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -2213,10 +2214,7 @@
       <c r="M27" s="3">
         <v>0</v>
       </c>
-      <c r="N27" s="1">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
+      <c r="N27" s="1"/>
       <c r="P27" s="3">
         <v>0</v>
       </c>
@@ -2247,16 +2245,16 @@
     </row>
     <row r="28" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2270,8 +2268,8 @@
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.2</v>
+        <f t="shared" ref="N28:N70" si="5">C28-D28*20-E28*0.8-F28*0.6-H28*5+I28*10+J28/300+G28/1.3</f>
+        <v>0.6</v>
       </c>
       <c r="P28" s="3">
         <v>0</v>
@@ -2303,16 +2301,16 @@
     </row>
     <row r="29" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="3">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2323,17 +2321,17 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" si="5"/>
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="P29" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q29" s="3">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
@@ -2344,11 +2342,11 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AA29" s="1">
         <f t="shared" si="2"/>
-        <v>-0.4</v>
+        <v>1.2</v>
       </c>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
@@ -2358,10 +2356,18 @@
       <c r="AG29" s="1"/>
     </row>
     <row r="30" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="A30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2370,13 +2376,19 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
       <c r="N30" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0.02</v>
+      </c>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
@@ -2385,10 +2397,12 @@
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
       <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
+      <c r="Z30" s="3">
+        <v>0</v>
+      </c>
       <c r="AA30" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
@@ -2398,13 +2412,53 @@
       <c r="AG30" s="1"/>
     </row>
     <row r="31" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
       <c r="N31" s="1">
         <f t="shared" si="5"/>
+        <v>-0.2</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="3">
         <v>0</v>
       </c>
       <c r="AA31" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
@@ -2414,13 +2468,53 @@
       <c r="AG31" s="1"/>
     </row>
     <row r="32" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
       <c r="N32" s="1">
         <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="3">
         <v>0</v>
       </c>
       <c r="AA32" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
@@ -2429,14 +2523,48 @@
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
     </row>
-    <row r="33" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
       <c r="N33" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="P33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4">
+        <v>0</v>
+      </c>
       <c r="AA33" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
@@ -2445,7 +2573,7 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
     </row>
-    <row r="34" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N34" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2461,7 +2589,7 @@
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
     </row>
-    <row r="35" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N35" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2477,7 +2605,7 @@
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
     </row>
-    <row r="36" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N36" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2493,7 +2621,7 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N37" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2509,7 +2637,7 @@
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
     </row>
-    <row r="38" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N38" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2525,7 +2653,7 @@
       <c r="AF38" s="1"/>
       <c r="AG38" s="1"/>
     </row>
-    <row r="39" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N39" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2541,7 +2669,7 @@
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
     </row>
-    <row r="40" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N40" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2557,7 +2685,7 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N41" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2573,7 +2701,7 @@
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
     </row>
-    <row r="42" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N42" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2589,7 +2717,7 @@
       <c r="AF42" s="1"/>
       <c r="AG42" s="1"/>
     </row>
-    <row r="43" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N43" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2605,7 +2733,7 @@
       <c r="AF43" s="1"/>
       <c r="AG43" s="1"/>
     </row>
-    <row r="44" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N44" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2621,7 +2749,7 @@
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
     </row>
-    <row r="45" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N45" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2637,7 +2765,7 @@
       <c r="AF45" s="1"/>
       <c r="AG45" s="1"/>
     </row>
-    <row r="46" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N46" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2653,7 +2781,7 @@
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
     </row>
-    <row r="47" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N47" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2669,7 +2797,7 @@
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
     </row>
-    <row r="48" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N48" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2989,9 +3117,54 @@
       <c r="AF67" s="1"/>
       <c r="AG67" s="1"/>
     </row>
-    <row r="68" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N68" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA68" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AE68" s="1"/>
+      <c r="AF68" s="1"/>
+      <c r="AG68" s="1"/>
+    </row>
+    <row r="69" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N69" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA69" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="1"/>
+      <c r="AE69" s="1"/>
+      <c r="AF69" s="1"/>
+      <c r="AG69" s="1"/>
+    </row>
+    <row r="70" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N70" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA70" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="1"/>
+      <c r="AG70" s="1"/>
+    </row>
     <row r="71" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="14:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3913,6 +4086,9 @@
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>